<commit_message>
Add task for 20-01
</commit_message>
<xml_diff>
--- a/Other/Task Tracking/Tracking.xlsx
+++ b/Other/Task Tracking/Tracking.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everything\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DO an\SVN_Team2\Other\Task Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Attendent check" sheetId="1" r:id="rId1"/>
@@ -77,8 +77,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[$-1010000]d/m/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="[$-1010409]d/m/yyyy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-1010409]d/m/yyyy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -170,23 +170,23 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,52 +479,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="6"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
@@ -541,38 +541,42 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
+      <c r="A12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+      <c r="A14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+      <c r="A15" s="7"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="A16" s="7"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="7"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="A18" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -587,13 +591,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="11" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="8" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
@@ -601,33 +605,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -638,11 +642,11 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
@@ -659,19 +663,19 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update task tracking va task trong tet
</commit_message>
<xml_diff>
--- a/Other/Task Tracking/Tracking.xlsx
+++ b/Other/Task Tracking/Tracking.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DO an\SVN_Team2\Other\Task Tracking\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Attendent check" sheetId="1" r:id="rId1"/>
     <sheet name="Deadline" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Attendent check</t>
   </si>
@@ -70,6 +65,12 @@
   </si>
   <si>
     <t>Usecase</t>
+  </si>
+  <si>
+    <t>23/01/04</t>
+  </si>
+  <si>
+    <t>23/01/14</t>
   </si>
 </sst>
 </file>
@@ -247,7 +248,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -282,7 +283,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -459,7 +460,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -469,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,9 +554,19 @@
       <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
@@ -589,10 +600,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,6 +690,23 @@
         <v>14</v>
       </c>
     </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:J3"/>

</xml_diff>